<commit_message>
updates to sret word selections & stratifications
balancing frequency & valence across +/negative words
</commit_message>
<xml_diff>
--- a/self_reference/emote_top_200_positive_negative_marked_RPA_DP.xlsx
+++ b/self_reference/emote_top_200_positive_negative_marked_RPA_DP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/AUERBACHLAB/Columbia/mbNF_MDD/REMIND/self_reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DB0C4D-3A9C-2C46-94D0-DCDA8EB4E27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C0834E-AB6E-E24A-850E-1947620C0602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="1820" windowWidth="27880" windowHeight="21300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="412">
   <si>
     <t>word</t>
   </si>
@@ -1836,7 +1836,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2124,7 +2124,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2134,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A225" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="H239" sqref="H239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4555,9 +4555,6 @@
       <c r="E139" s="6">
         <v>5.8</v>
       </c>
-      <c r="F139" s="2" t="s">
-        <v>411</v>
-      </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
@@ -4612,9 +4609,6 @@
       <c r="E142" s="6">
         <v>5.47</v>
       </c>
-      <c r="F142" s="2" t="s">
-        <v>411</v>
-      </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
@@ -6052,7 +6046,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>405</v>
       </c>
@@ -6069,7 +6063,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>405</v>
       </c>
@@ -6086,7 +6080,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>405</v>
       </c>
@@ -6103,7 +6097,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>405</v>
       </c>
@@ -6120,7 +6114,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>405</v>
       </c>
@@ -6137,7 +6131,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>405</v>
       </c>
@@ -6154,7 +6148,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>405</v>
       </c>
@@ -6171,7 +6165,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>405</v>
       </c>
@@ -6188,7 +6182,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>405</v>
       </c>
@@ -6205,7 +6199,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>405</v>
       </c>
@@ -6222,7 +6216,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>405</v>
       </c>
@@ -6239,7 +6233,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>405</v>
       </c>
@@ -6256,7 +6250,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>405</v>
       </c>
@@ -6273,7 +6267,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>405</v>
       </c>
@@ -6289,8 +6283,11 @@
       <c r="E238" s="5">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F238" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>405</v>
       </c>
@@ -6307,7 +6304,7 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>405</v>
       </c>

</xml_diff>